<commit_message>
UI and bug updates
</commit_message>
<xml_diff>
--- a/loadtests/WindowsHello_vs_FaceTrack.xlsx
+++ b/loadtests/WindowsHello_vs_FaceTrack.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kartikey/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kartikey/Desktop/ML_Projects/attendance-app-with-facial-recognition/loadtests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D3ACC8-28AB-EA42-A555-465950DD8C10}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68839AF-E37D-484E-81C8-75FF12620FAF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>Windows Hello</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>✅ 良好（IRセンサーを使用）</t>
-  </si>
-  <si>
-    <t>❌ マスク着用者は認証不可</t>
   </si>
   <si>
     <t>✅ メガネや多少の外見変化に対応</t>
@@ -266,6 +263,18 @@
   </si>
   <si>
     <t>❌ 標準Webカメラは弱い；IR対応カメラが必要</t>
+  </si>
+  <si>
+    <t>サングラス</t>
+  </si>
+  <si>
+    <t>✅ サングラスを着用していても認識可能</t>
+  </si>
+  <si>
+    <t>❌ サングラスを着用者は認証不可</t>
+  </si>
+  <si>
+    <t>❌ マスクを着用者は認証不可</t>
   </si>
 </sst>
 </file>
@@ -617,6 +626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -677,7 +687,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -764,8 +773,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A6C292-E314-6842-8E75-BC4F2B9F98A5}" name="Table1" displayName="Table1" ref="A1:C22" totalsRowShown="0" tableBorderDxfId="3">
-  <autoFilter ref="A1:C22" xr:uid="{2E5917AA-E349-444C-A056-9CE0C8DF5A5C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A6C292-E314-6842-8E75-BC4F2B9F98A5}" name="Table1" displayName="Table1" ref="A1:C23" totalsRowShown="0" tableBorderDxfId="3">
+  <autoFilter ref="A1:C23" xr:uid="{2E5917AA-E349-444C-A056-9CE0C8DF5A5C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{10BF3855-F13F-B747-99A0-6AAAE811C0F5}" name="機能 / 基準" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{B6BCE1DB-A075-654E-AF29-2DD1871EB90A}" name="Windows Hello" dataDxfId="1"/>
@@ -1096,11 +1105,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1120,10 +1129,10 @@
       <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="35"/>
+      <c r="E1" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="16" customHeight="1" thickTop="1">
       <c r="A2" s="5" t="s">
@@ -1133,15 +1142,15 @@
         <v>20</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="18"/>
+        <v>35</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10">
@@ -1152,13 +1161,13 @@
         <v>21</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21"/>
+        <v>36</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="22"/>
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10">
@@ -1169,13 +1178,13 @@
         <v>22</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21"/>
+        <v>37</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22"/>
       <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10">
@@ -1186,13 +1195,13 @@
         <v>23</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21"/>
+        <v>65</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="22"/>
       <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10">
@@ -1200,33 +1209,33 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="21"/>
+        <v>49</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="22"/>
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="22"/>
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10">
@@ -1234,16 +1243,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="21"/>
+        <v>64</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="22"/>
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10">
@@ -1251,16 +1260,16 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
+        <v>62</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22"/>
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10">
@@ -1268,16 +1277,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="21"/>
+        <v>38</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="22"/>
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10">
@@ -1285,16 +1294,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="24"/>
+        <v>39</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
       <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:10">
@@ -1302,10 +1311,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -1319,10 +1328,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -1336,13 +1345,13 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="15"/>
-      <c r="F14" s="36"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
@@ -1353,10 +1362,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -1370,10 +1379,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1387,10 +1396,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -1404,10 +1413,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -1421,10 +1430,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -1435,13 +1444,13 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -1452,13 +1461,13 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -1469,13 +1478,13 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -1485,97 +1494,103 @@
       <c r="J22" s="15"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-    </row>
-    <row r="24" spans="1:10" ht="16" thickBot="1"/>
-    <row r="25" spans="1:10">
-      <c r="A25" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="27"/>
-    </row>
+      <c r="A23" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="1:10" ht="16" thickBot="1"/>
     <row r="26" spans="1:10">
-      <c r="A26" s="28"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="30"/>
+      <c r="A26" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="28"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="30"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="31"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="28"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="30"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="31"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="28"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="30"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="31"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="28"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="30"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="31"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="28"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="30"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="30"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="31"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="28"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="30"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="31"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="28"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="30"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="31"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="28"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="30"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="31"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="28"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="30"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="31"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="28"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="30"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="31"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="28"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="30"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="31"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="28"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="30"/>
-    </row>
-    <row r="40" spans="1:3" ht="16" thickBot="1">
-      <c r="A40" s="31"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="33"/>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+      <c r="A39" s="29"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="31"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="29"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="31"/>
+    </row>
+    <row r="41" spans="1:3" ht="16" thickBot="1">
+      <c r="A41" s="32"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="34"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1"/>
@@ -1622,14 +1637,19 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="E2:I11"/>
-    <mergeCell ref="A25:C40"/>
+    <mergeCell ref="A26:C41"/>
     <mergeCell ref="E1:F1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:C23">
-    <cfRule type="colorScale" priority="15">
+  <conditionalFormatting sqref="A2:C24">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1637,7 +1657,7 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1647,6 +1667,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>